<commit_message>
Fixed offset well position problem.
</commit_message>
<xml_diff>
--- a/worklist_template0821.xlsx
+++ b/worklist_template0821.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabewilson/Desktop/worklist_generation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivint\OneDrive\Desktop\Kelly_Lab\.venv\worklist_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C475920-8B4E-6047-BA79-7E89E10A5C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDA46E5-548B-4E5B-B6E0-B58ECD1256FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17100" xr2:uid="{12DA0CF9-A1F3-4B47-B73A-18ED55D7EBC7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{12DA0CF9-A1F3-4B47-B73A-18ED55D7EBC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -871,11 +871,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A45856-9C0F-D140-AD60-2AFFFFA45290}">
   <dimension ref="A1:AV63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q22" zoomScale="83" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AL53" sqref="AL53"/>
+    <sheetView tabSelected="1" topLeftCell="AH8" zoomScale="52" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AV35" sqref="AV35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
@@ -898,7 +898,7 @@
     <col min="43" max="45" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -954,7 +954,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1004,7 +1004,7 @@
       <c r="AR2" s="12"/>
       <c r="AS2" s="11"/>
     </row>
-    <row r="3" spans="1:48" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:48" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="AV3" s="30"/>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="D4" s="3"/>
@@ -1131,7 +1131,7 @@
       <c r="AU4" s="30"/>
       <c r="AV4" s="30"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1258,7 +1258,7 @@
       <c r="AU5" s="30"/>
       <c r="AV5" s="30"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A6" s="13" t="s">
         <v>50</v>
       </c>
@@ -1339,7 +1339,7 @@
       <c r="AU6" s="30"/>
       <c r="AV6" s="30"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D7" t="s">
         <v>18</v>
       </c>
@@ -1442,7 +1442,7 @@
       <c r="AU7" s="30"/>
       <c r="AV7" s="30"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D8" t="s">
         <v>19</v>
       </c>
@@ -1545,7 +1545,7 @@
       <c r="AU8" s="30"/>
       <c r="AV8" s="30"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
         <v>20</v>
       </c>
@@ -1638,7 +1638,7 @@
       <c r="AU9" s="30"/>
       <c r="AV9" s="30"/>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D10" t="s">
         <v>21</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="AU10" s="30"/>
       <c r="AV10" s="30"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
         <v>22</v>
       </c>
@@ -1824,7 +1824,7 @@
       <c r="AU11" s="30"/>
       <c r="AV11" s="30"/>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D12" t="s">
         <v>23</v>
       </c>
@@ -1917,7 +1917,7 @@
       <c r="AU12" s="30"/>
       <c r="AV12" s="30"/>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D13" t="s">
         <v>24</v>
       </c>
@@ -2010,7 +2010,7 @@
       <c r="AU13" s="30"/>
       <c r="AV13" s="30"/>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D14" t="s">
         <v>25</v>
       </c>
@@ -2103,7 +2103,7 @@
       <c r="AU14" s="30"/>
       <c r="AV14" s="30"/>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
         <v>26</v>
       </c>
@@ -2194,7 +2194,7 @@
       <c r="AR15" s="12"/>
       <c r="AS15" s="11"/>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D16" t="s">
         <v>27</v>
       </c>
@@ -2285,7 +2285,7 @@
       <c r="AR16" s="12"/>
       <c r="AS16" s="11"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D17" t="s">
         <v>28</v>
       </c>
@@ -2376,7 +2376,7 @@
       <c r="AR17" s="12"/>
       <c r="AS17" s="11"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D18" t="s">
         <v>29</v>
       </c>
@@ -2467,7 +2467,7 @@
       <c r="AR18" s="12"/>
       <c r="AS18" s="11"/>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D19" t="s">
         <v>30</v>
       </c>
@@ -2558,7 +2558,7 @@
       <c r="AR19" s="12"/>
       <c r="AS19" s="11"/>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D20" t="s">
         <v>31</v>
       </c>
@@ -2649,7 +2649,7 @@
       <c r="AR20" s="12"/>
       <c r="AS20" s="11"/>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D21" t="s">
         <v>32</v>
       </c>
@@ -2740,7 +2740,7 @@
       <c r="AR21" s="12"/>
       <c r="AS21" s="11"/>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="D22" s="3"/>
@@ -2811,7 +2811,7 @@
       <c r="AR22" s="12"/>
       <c r="AS22" s="11"/>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
@@ -2936,7 +2936,7 @@
       <c r="AR23" s="12"/>
       <c r="AS23" s="11"/>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="D24" t="s">
@@ -3009,7 +3009,7 @@
       <c r="AR24" s="12"/>
       <c r="AS24" s="11"/>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D25" t="s">
         <v>18</v>
       </c>
@@ -3080,7 +3080,7 @@
       <c r="AR25" s="12"/>
       <c r="AS25" s="11"/>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D26" t="s">
         <v>19</v>
       </c>
@@ -3151,7 +3151,7 @@
       <c r="AR26" s="12"/>
       <c r="AS26" s="11"/>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D27" t="s">
         <v>20</v>
       </c>
@@ -3222,7 +3222,7 @@
       <c r="AR27" s="12"/>
       <c r="AS27" s="11"/>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D28" t="s">
         <v>21</v>
       </c>
@@ -3293,7 +3293,7 @@
       <c r="AR28" s="12"/>
       <c r="AS28" s="11"/>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D29" t="s">
         <v>22</v>
       </c>
@@ -3364,7 +3364,7 @@
       <c r="AR29" s="12"/>
       <c r="AS29" s="11"/>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D30" t="s">
         <v>23</v>
       </c>
@@ -3435,7 +3435,7 @@
       <c r="AR30" s="12"/>
       <c r="AS30" s="11"/>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D31" t="s">
         <v>24</v>
       </c>
@@ -3506,7 +3506,7 @@
       <c r="AR31" s="12"/>
       <c r="AS31" s="11"/>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D32" t="s">
         <v>25</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D33" t="s">
         <v>26</v>
       </c>
@@ -3657,10 +3657,10 @@
         <v>1</v>
       </c>
       <c r="AS33" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D34" t="s">
         <v>27</v>
       </c>
@@ -3707,7 +3707,7 @@
       <c r="AR34" s="12"/>
       <c r="AS34" s="11"/>
     </row>
-    <row r="35" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D35" t="s">
         <v>28</v>
       </c>
@@ -3754,7 +3754,7 @@
       <c r="AR35" s="12"/>
       <c r="AS35" s="11"/>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D36" t="s">
         <v>29</v>
       </c>
@@ -3801,7 +3801,7 @@
       <c r="AR36" s="12"/>
       <c r="AS36" s="11"/>
     </row>
-    <row r="37" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D37" t="s">
         <v>30</v>
       </c>
@@ -3848,7 +3848,7 @@
       <c r="AR37" s="12"/>
       <c r="AS37" s="11"/>
     </row>
-    <row r="38" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D38" t="s">
         <v>31</v>
       </c>
@@ -3895,7 +3895,7 @@
       <c r="AR38" s="12"/>
       <c r="AS38" s="11"/>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D39" t="s">
         <v>32</v>
       </c>
@@ -3942,7 +3942,7 @@
       <c r="AR39" s="12"/>
       <c r="AS39" s="11"/>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="D40" s="3"/>
@@ -3989,7 +3989,7 @@
       <c r="AR40" s="12"/>
       <c r="AS40" s="11"/>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A41" s="4" t="s">
         <v>14</v>
       </c>
@@ -4090,7 +4090,7 @@
       <c r="AR41" s="12"/>
       <c r="AS41" s="11"/>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="D42" t="s">
@@ -4139,7 +4139,7 @@
       <c r="AR42" s="12"/>
       <c r="AS42" s="11"/>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D43" t="s">
         <v>18</v>
       </c>
@@ -4186,7 +4186,7 @@
       <c r="AR43" s="12"/>
       <c r="AS43" s="11"/>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D44" t="s">
         <v>19</v>
       </c>
@@ -4233,7 +4233,7 @@
       <c r="AR44" s="12"/>
       <c r="AS44" s="11"/>
     </row>
-    <row r="45" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D45" t="s">
         <v>20</v>
       </c>
@@ -4280,7 +4280,7 @@
       <c r="AR45" s="12"/>
       <c r="AS45" s="11"/>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D46" t="s">
         <v>21</v>
       </c>
@@ -4327,7 +4327,7 @@
       <c r="AR46" s="12"/>
       <c r="AS46" s="11"/>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D47" t="s">
         <v>22</v>
       </c>
@@ -4374,7 +4374,7 @@
       <c r="AR47" s="12"/>
       <c r="AS47" s="11"/>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D48" t="s">
         <v>23</v>
       </c>
@@ -4421,7 +4421,7 @@
       <c r="AR48" s="12"/>
       <c r="AS48" s="11"/>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D49" t="s">
         <v>24</v>
       </c>
@@ -4468,7 +4468,7 @@
       <c r="AR49" s="12"/>
       <c r="AS49" s="11"/>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D50" t="s">
         <v>25</v>
       </c>
@@ -4515,7 +4515,7 @@
       <c r="AR50" s="12"/>
       <c r="AS50" s="11"/>
     </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D51" t="s">
         <v>26</v>
       </c>
@@ -4562,7 +4562,7 @@
       <c r="AR51" s="20"/>
       <c r="AS51" s="21"/>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D52" t="s">
         <v>27</v>
       </c>
@@ -4591,7 +4591,7 @@
       <c r="AA52" s="10"/>
       <c r="AB52" s="9"/>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D53" t="s">
         <v>28</v>
       </c>
@@ -4640,7 +4640,7 @@
       </c>
       <c r="AN53" s="31"/>
     </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D54" t="s">
         <v>29</v>
       </c>
@@ -4680,7 +4680,7 @@
       <c r="AM54" s="31"/>
       <c r="AN54" s="31"/>
     </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D55" t="s">
         <v>30</v>
       </c>
@@ -4725,7 +4725,7 @@
       <c r="AM55" s="31"/>
       <c r="AN55" s="31"/>
     </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D56" t="s">
         <v>31</v>
       </c>
@@ -4759,7 +4759,7 @@
       <c r="AK56" s="34"/>
       <c r="AL56" s="37"/>
     </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D57" t="s">
         <v>32</v>
       </c>
@@ -4795,7 +4795,7 @@
       <c r="AM57" s="23"/>
       <c r="AN57" s="23"/>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="D58" s="3"/>
@@ -4838,7 +4838,7 @@
       <c r="AM58" s="23"/>
       <c r="AN58" s="23"/>
     </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.4">
       <c r="AE59" s="10"/>
       <c r="AJ59" s="30"/>
       <c r="AK59" s="23"/>
@@ -4846,19 +4846,19 @@
       <c r="AM59" s="23"/>
       <c r="AN59" s="23"/>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.4">
       <c r="AE60" s="10"/>
       <c r="AJ60" s="30"/>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.4">
       <c r="AE61" s="10"/>
       <c r="AJ61" s="30"/>
     </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.4">
       <c r="AE62" s="10"/>
       <c r="AJ62" s="30"/>
     </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.4">
       <c r="AE63" s="10"/>
       <c r="AJ63" s="30"/>
     </row>
@@ -4903,7 +4903,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New processor implemented including switching 'between' column to 'samples per between block.
</commit_message>
<xml_diff>
--- a/worklist_template0821.xlsx
+++ b/worklist_template0821.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivint\OneDrive\Desktop\Kelly_Lab\.venv\worklist_git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01c1829094dbd390/Desktop/Kelly_Lab/.venv/worklist_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDA46E5-548B-4E5B-B6E0-B58ECD1256FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{60CEAB5E-1B2A-42D8-B1E6-AC461F9ED1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBE19B2A-825C-432F-9012-188A1843CB6B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{12DA0CF9-A1F3-4B47-B73A-18ED55D7EBC7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="73">
   <si>
     <t>Notebook code:</t>
   </si>
@@ -186,67 +186,76 @@
     <t>Nothing</t>
   </si>
   <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>TrueBlank</t>
+  </si>
+  <si>
+    <t>D:/data/Ximena/Gonda0821</t>
+  </si>
+  <si>
+    <t>D:/method/Chao/something</t>
+  </si>
+  <si>
+    <t>DIA20ng</t>
+  </si>
+  <si>
+    <t>LC method file name:</t>
+  </si>
+  <si>
+    <t>MS method file name:</t>
+  </si>
+  <si>
+    <t>C:/data/Ximena/Gonda</t>
+  </si>
+  <si>
+    <t>lcmethodpath</t>
+  </si>
+  <si>
+    <t>lcmethodfilename</t>
+  </si>
+  <si>
+    <t>lcmethodshort_dry</t>
+  </si>
+  <si>
+    <t>QC before</t>
+  </si>
+  <si>
+    <t>QC after</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>TrueBlank condition number</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Frequency of QC blocks:</t>
+  </si>
+  <si>
+    <t>QC per block</t>
+  </si>
+  <si>
+    <t>blueplate</t>
+  </si>
+  <si>
+    <t>greenplate</t>
+  </si>
+  <si>
+    <t>redplate</t>
+  </si>
+  <si>
+    <t>QC per between block</t>
+  </si>
+  <si>
     <t>2 column</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Gonda</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>TrueBlank</t>
-  </si>
-  <si>
-    <t>D:/data/Ximena/Gonda0821</t>
-  </si>
-  <si>
-    <t>D:/method/Chao/something</t>
-  </si>
-  <si>
-    <t>DIA20ng</t>
-  </si>
-  <si>
-    <t>LC method file name:</t>
-  </si>
-  <si>
-    <t>MS method file name:</t>
-  </si>
-  <si>
-    <t>C:/data/Ximena/Gonda</t>
-  </si>
-  <si>
-    <t>lcmethodpath</t>
-  </si>
-  <si>
-    <t>lcmethodfilename</t>
-  </si>
-  <si>
-    <t>lcmethodshort_dry</t>
-  </si>
-  <si>
-    <t>QC before</t>
-  </si>
-  <si>
-    <t>QC after</t>
-  </si>
-  <si>
-    <t>QC between</t>
-  </si>
-  <si>
-    <t>QC</t>
-  </si>
-  <si>
-    <t>TrueBlank condition number</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>1-32</t>
   </si>
 </sst>
 </file>
@@ -450,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -511,6 +520,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -871,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A45856-9C0F-D140-AD60-2AFFFFA45290}">
   <dimension ref="A1:AV63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH8" zoomScale="52" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AV35" sqref="AV35"/>
+    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -889,13 +904,14 @@
     <col min="34" max="34" width="38.1640625" customWidth="1"/>
     <col min="35" max="35" width="15.33203125" customWidth="1"/>
     <col min="36" max="36" width="21.1640625" customWidth="1"/>
-    <col min="37" max="37" width="20.83203125" customWidth="1"/>
+    <col min="37" max="37" width="23.08203125" customWidth="1"/>
     <col min="38" max="38" width="30.83203125" customWidth="1"/>
     <col min="39" max="39" width="14.83203125" customWidth="1"/>
     <col min="40" max="40" width="25.83203125" customWidth="1"/>
     <col min="41" max="41" width="30.1640625" customWidth="1"/>
     <col min="42" max="42" width="21.83203125" customWidth="1"/>
-    <col min="43" max="45" width="15.33203125" customWidth="1"/>
+    <col min="43" max="44" width="15.33203125" customWidth="1"/>
+    <col min="45" max="45" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.4">
@@ -924,7 +940,7 @@
         <v>6</v>
       </c>
       <c r="AJ1" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AK1" s="5" t="s">
         <v>7</v>
@@ -936,7 +952,7 @@
         <v>9</v>
       </c>
       <c r="AN1" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AO1" s="28" t="s">
         <v>10</v>
@@ -945,13 +961,13 @@
         <v>11</v>
       </c>
       <c r="AQ1" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AR1" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AS1" s="4" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.4">
@@ -965,34 +981,34 @@
         <v>1</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF2" s="7">
         <v>1</v>
       </c>
       <c r="AG2" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI2" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ2" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN2" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL2" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN2" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO2" s="29">
         <v>1</v>
@@ -1009,40 +1025,40 @@
         <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="AD3" s="12">
         <v>2</v>
       </c>
       <c r="AE3" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF3" s="7">
         <v>2</v>
       </c>
       <c r="AG3" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH3" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI3" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ3" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN3" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL3" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM3" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN3" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO3" s="29">
         <v>1</v>
@@ -1053,10 +1069,10 @@
       <c r="AQ3" s="12"/>
       <c r="AR3" s="12"/>
       <c r="AS3" s="11"/>
-      <c r="AU3" s="30" t="s">
+      <c r="AU3" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="AV3" s="30"/>
+      <c r="AV3" s="32"/>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
@@ -1090,34 +1106,34 @@
         <v>3</v>
       </c>
       <c r="AE4" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF4" s="7">
         <v>3</v>
       </c>
       <c r="AG4" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH4" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI4" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ4" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN4" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM4" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN4" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO4" s="29">
         <v>1</v>
@@ -1128,8 +1144,8 @@
       <c r="AQ4" s="12"/>
       <c r="AR4" s="12"/>
       <c r="AS4" s="11"/>
-      <c r="AU4" s="30"/>
-      <c r="AV4" s="30"/>
+      <c r="AU4" s="32"/>
+      <c r="AV4" s="32"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
@@ -1217,34 +1233,34 @@
         <v>4</v>
       </c>
       <c r="AE5" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF5" s="7">
         <v>4</v>
       </c>
       <c r="AG5" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH5" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI5" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK5" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN5" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM5" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN5" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO5" s="29">
         <v>1</v>
@@ -1255,15 +1271,15 @@
       <c r="AQ5" s="12"/>
       <c r="AR5" s="12"/>
       <c r="AS5" s="11"/>
-      <c r="AU5" s="30"/>
-      <c r="AV5" s="30"/>
+      <c r="AU5" s="32"/>
+      <c r="AV5" s="32"/>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A6" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -1298,34 +1314,34 @@
         <v>5</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF6" s="7">
         <v>5</v>
       </c>
       <c r="AG6" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI6" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ6" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN6" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM6" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN6" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO6" s="29">
         <v>1</v>
@@ -1336,8 +1352,8 @@
       <c r="AQ6" s="12"/>
       <c r="AR6" s="12"/>
       <c r="AS6" s="11"/>
-      <c r="AU6" s="30"/>
-      <c r="AV6" s="30"/>
+      <c r="AU6" s="32"/>
+      <c r="AV6" s="32"/>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D7" t="s">
@@ -1401,34 +1417,34 @@
         <v>6</v>
       </c>
       <c r="AE7" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF7" s="7">
         <v>6</v>
       </c>
       <c r="AG7" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH7" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI7" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ7" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK7" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN7" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL7" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM7" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN7" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO7" s="29">
         <v>1</v>
@@ -1439,8 +1455,8 @@
       <c r="AQ7" s="12"/>
       <c r="AR7" s="12"/>
       <c r="AS7" s="11"/>
-      <c r="AU7" s="30"/>
-      <c r="AV7" s="30"/>
+      <c r="AU7" s="32"/>
+      <c r="AV7" s="32"/>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D8" t="s">
@@ -1504,34 +1520,34 @@
         <v>7</v>
       </c>
       <c r="AE8" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF8" s="7">
         <v>7</v>
       </c>
       <c r="AG8" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH8" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI8" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ8" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN8" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL8" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN8" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO8" s="29">
         <v>1</v>
@@ -1542,8 +1558,8 @@
       <c r="AQ8" s="12"/>
       <c r="AR8" s="12"/>
       <c r="AS8" s="11"/>
-      <c r="AU8" s="30"/>
-      <c r="AV8" s="30"/>
+      <c r="AU8" s="32"/>
+      <c r="AV8" s="32"/>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
@@ -1597,34 +1613,34 @@
         <v>8</v>
       </c>
       <c r="AE9" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF9" s="7">
         <v>8</v>
       </c>
       <c r="AG9" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH9" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI9" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ9" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN9" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL9" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM9" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN9" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO9" s="29">
         <v>1</v>
@@ -1635,8 +1651,8 @@
       <c r="AQ9" s="12"/>
       <c r="AR9" s="12"/>
       <c r="AS9" s="11"/>
-      <c r="AU9" s="30"/>
-      <c r="AV9" s="30"/>
+      <c r="AU9" s="32"/>
+      <c r="AV9" s="32"/>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D10" t="s">
@@ -1690,34 +1706,34 @@
         <v>9</v>
       </c>
       <c r="AE10" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF10" s="7">
         <v>9</v>
       </c>
       <c r="AG10" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH10" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI10" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ10" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN10" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL10" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM10" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN10" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO10" s="29">
         <v>1</v>
@@ -1728,8 +1744,8 @@
       <c r="AQ10" s="12"/>
       <c r="AR10" s="12"/>
       <c r="AS10" s="11"/>
-      <c r="AU10" s="30"/>
-      <c r="AV10" s="30"/>
+      <c r="AU10" s="32"/>
+      <c r="AV10" s="32"/>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
@@ -1783,34 +1799,34 @@
         <v>10</v>
       </c>
       <c r="AE11" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF11" s="7">
         <v>10</v>
       </c>
       <c r="AG11" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH11" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI11" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ11" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN11" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL11" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM11" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN11" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO11" s="29">
         <v>1</v>
@@ -1821,8 +1837,8 @@
       <c r="AQ11" s="12"/>
       <c r="AR11" s="12"/>
       <c r="AS11" s="11"/>
-      <c r="AU11" s="30"/>
-      <c r="AV11" s="30"/>
+      <c r="AU11" s="32"/>
+      <c r="AV11" s="32"/>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D12" t="s">
@@ -1876,34 +1892,34 @@
         <v>11</v>
       </c>
       <c r="AE12" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF12" s="7">
         <v>11</v>
       </c>
       <c r="AG12" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH12" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI12" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ12" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN12" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL12" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM12" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN12" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO12" s="29">
         <v>1</v>
@@ -1914,8 +1930,8 @@
       <c r="AQ12" s="12"/>
       <c r="AR12" s="12"/>
       <c r="AS12" s="11"/>
-      <c r="AU12" s="30"/>
-      <c r="AV12" s="30"/>
+      <c r="AU12" s="32"/>
+      <c r="AV12" s="32"/>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D13" t="s">
@@ -1969,34 +1985,34 @@
         <v>12</v>
       </c>
       <c r="AE13" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF13" s="7">
         <v>12</v>
       </c>
       <c r="AG13" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH13" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI13" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ13" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN13" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL13" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM13" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN13" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO13" s="29">
         <v>1</v>
@@ -2007,8 +2023,8 @@
       <c r="AQ13" s="12"/>
       <c r="AR13" s="12"/>
       <c r="AS13" s="11"/>
-      <c r="AU13" s="30"/>
-      <c r="AV13" s="30"/>
+      <c r="AU13" s="32"/>
+      <c r="AV13" s="32"/>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D14" t="s">
@@ -2062,34 +2078,34 @@
         <v>13</v>
       </c>
       <c r="AE14" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF14" s="7">
         <v>13</v>
       </c>
       <c r="AG14" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH14" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI14" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ14" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN14" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL14" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM14" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN14" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO14" s="29">
         <v>1</v>
@@ -2100,8 +2116,8 @@
       <c r="AQ14" s="12"/>
       <c r="AR14" s="12"/>
       <c r="AS14" s="11"/>
-      <c r="AU14" s="30"/>
-      <c r="AV14" s="30"/>
+      <c r="AU14" s="32"/>
+      <c r="AV14" s="32"/>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
@@ -2155,34 +2171,34 @@
         <v>14</v>
       </c>
       <c r="AE15" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF15" s="7">
         <v>14</v>
       </c>
       <c r="AG15" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH15" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI15" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ15" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK15" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN15" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL15" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM15" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN15" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO15" s="29">
         <v>1</v>
@@ -2246,34 +2262,34 @@
         <v>15</v>
       </c>
       <c r="AE16" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF16" s="7">
         <v>15</v>
       </c>
       <c r="AG16" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH16" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI16" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ16" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN16" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL16" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM16" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN16" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO16" s="29">
         <v>1</v>
@@ -2337,34 +2353,34 @@
         <v>16</v>
       </c>
       <c r="AE17" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF17" s="7">
         <v>16</v>
       </c>
       <c r="AG17" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH17" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI17" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ17" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN17" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL17" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM17" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN17" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO17" s="29">
         <v>1</v>
@@ -2428,34 +2444,34 @@
         <v>17</v>
       </c>
       <c r="AE18" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF18" s="7">
         <v>17</v>
       </c>
       <c r="AG18" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH18" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI18" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ18" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN18" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL18" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM18" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN18" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO18" s="29">
         <v>1</v>
@@ -2519,34 +2535,34 @@
         <v>18</v>
       </c>
       <c r="AE19" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF19" s="7">
         <v>18</v>
       </c>
       <c r="AG19" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH19" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI19" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ19" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN19" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL19" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM19" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN19" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO19" s="29">
         <v>1</v>
@@ -2610,34 +2626,34 @@
         <v>19</v>
       </c>
       <c r="AE20" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF20" s="7">
         <v>19</v>
       </c>
       <c r="AG20" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH20" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI20" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ20" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN20" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL20" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM20" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN20" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO20" s="29">
         <v>1</v>
@@ -2701,34 +2717,34 @@
         <v>20</v>
       </c>
       <c r="AE21" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF21" s="7">
         <v>20</v>
       </c>
       <c r="AG21" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH21" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI21" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ21" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK21" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM21" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN21" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL21" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM21" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN21" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO21" s="29">
         <v>1</v>
@@ -2772,34 +2788,34 @@
         <v>21</v>
       </c>
       <c r="AE22" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF22" s="7">
         <v>21</v>
       </c>
       <c r="AG22" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH22" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI22" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ22" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK22" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM22" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN22" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL22" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM22" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN22" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO22" s="29">
         <v>1</v>
@@ -2897,34 +2913,34 @@
         <v>22</v>
       </c>
       <c r="AE23" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF23" s="7">
         <v>22</v>
       </c>
       <c r="AG23" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH23" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI23" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ23" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK23" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN23" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL23" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM23" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN23" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO23" s="29">
         <v>1</v>
@@ -2937,8 +2953,12 @@
       <c r="AS23" s="11"/>
     </row>
     <row r="24" spans="1:45" x14ac:dyDescent="0.4">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="D24" t="s">
         <v>17</v>
       </c>
@@ -2970,34 +2990,34 @@
         <v>23</v>
       </c>
       <c r="AE24" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF24" s="7">
         <v>23</v>
       </c>
       <c r="AG24" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH24" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI24" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ24" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK24" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL24" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM24" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN24" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL24" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM24" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN24" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO24" s="29">
         <v>1</v>
@@ -3041,34 +3061,34 @@
         <v>24</v>
       </c>
       <c r="AE25" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF25" s="7">
         <v>24</v>
       </c>
       <c r="AG25" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH25" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI25" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ25" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK25" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL25" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM25" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN25" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL25" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM25" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN25" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO25" s="29">
         <v>1</v>
@@ -3112,34 +3132,34 @@
         <v>25</v>
       </c>
       <c r="AE26" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF26" s="7">
         <v>25</v>
       </c>
       <c r="AG26" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH26" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI26" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ26" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK26" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM26" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN26" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL26" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM26" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN26" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO26" s="29">
         <v>1</v>
@@ -3183,34 +3203,34 @@
         <v>26</v>
       </c>
       <c r="AE27" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF27" s="7">
         <v>26</v>
       </c>
       <c r="AG27" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH27" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI27" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ27" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL27" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN27" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL27" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM27" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN27" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO27" s="29">
         <v>1</v>
@@ -3254,34 +3274,34 @@
         <v>27</v>
       </c>
       <c r="AE28" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF28" s="7">
         <v>27</v>
       </c>
       <c r="AG28" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH28" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI28" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ28" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK28" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL28" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM28" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN28" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL28" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM28" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN28" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO28" s="29">
         <v>1</v>
@@ -3325,34 +3345,34 @@
         <v>28</v>
       </c>
       <c r="AE29" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF29" s="7">
         <v>28</v>
       </c>
       <c r="AG29" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH29" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI29" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ29" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK29" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM29" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN29" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL29" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM29" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN29" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO29" s="29">
         <v>1</v>
@@ -3396,34 +3416,34 @@
         <v>29</v>
       </c>
       <c r="AE30" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF30" s="7">
         <v>29</v>
       </c>
       <c r="AG30" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH30" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI30" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ30" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK30" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL30" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM30" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN30" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL30" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM30" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN30" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO30" s="29">
         <v>1</v>
@@ -3467,34 +3487,34 @@
         <v>30</v>
       </c>
       <c r="AE31" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AF31" s="7">
         <v>30</v>
       </c>
       <c r="AG31" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH31" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI31" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ31" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK31" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL31" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM31" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN31" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL31" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM31" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN31" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO31" s="29">
         <v>1</v>
@@ -3538,34 +3558,34 @@
         <v>31</v>
       </c>
       <c r="AE32" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF32" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AG32" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH32" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI32" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ32" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK32" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL32" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM32" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN32" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL32" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM32" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN32" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO32" s="29">
         <v>3</v>
@@ -3580,7 +3600,7 @@
         <v>3</v>
       </c>
       <c r="AS32" s="11">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.4">
@@ -3615,40 +3635,40 @@
         <v>32</v>
       </c>
       <c r="AE33" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF33" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG33" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH33" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AF33" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG33" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH33" s="8" t="s">
-        <v>55</v>
-      </c>
       <c r="AI33" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ33" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK33" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL33" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM33" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN33" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="AL33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM33" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN33" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AO33" s="29">
         <v>1</v>
       </c>
       <c r="AP33" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="AQ33" s="12">
         <v>1</v>
@@ -4091,8 +4111,12 @@
       <c r="AS41" s="11"/>
     </row>
     <row r="42" spans="1:45" x14ac:dyDescent="0.4">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
+      <c r="A42" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>69</v>
+      </c>
       <c r="D42" t="s">
         <v>17</v>
       </c>
@@ -4619,10 +4643,10 @@
       <c r="Z53" s="10"/>
       <c r="AA53" s="10"/>
       <c r="AB53" s="9"/>
-      <c r="AE53" s="30" t="s">
+      <c r="AE53" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="AF53" s="30"/>
+      <c r="AF53" s="32"/>
       <c r="AH53" s="1" t="s">
         <v>35</v>
       </c>
@@ -4633,12 +4657,12 @@
         <v>37</v>
       </c>
       <c r="AL53" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="AM53" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM53" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="AN53" s="31"/>
+      <c r="AN53" s="33"/>
     </row>
     <row r="54" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D54" t="s">
@@ -4668,8 +4692,8 @@
       <c r="Z54" s="10"/>
       <c r="AA54" s="10"/>
       <c r="AB54" s="9"/>
-      <c r="AE54" s="30"/>
-      <c r="AF54" s="30"/>
+      <c r="AE54" s="32"/>
+      <c r="AF54" s="32"/>
       <c r="AH54" s="1" t="s">
         <v>39</v>
       </c>
@@ -4677,8 +4701,8 @@
       <c r="AK54" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AM54" s="31"/>
-      <c r="AN54" s="31"/>
+      <c r="AM54" s="33"/>
+      <c r="AN54" s="33"/>
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D55" t="s">
@@ -4708,22 +4732,22 @@
       <c r="Z55" s="10"/>
       <c r="AA55" s="10"/>
       <c r="AB55" s="9"/>
-      <c r="AE55" s="30"/>
-      <c r="AF55" s="30"/>
-      <c r="AH55" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI55" s="35">
+      <c r="AE55" s="32"/>
+      <c r="AF55" s="32"/>
+      <c r="AH55" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI55" s="37">
         <v>32</v>
       </c>
-      <c r="AK55" s="32" t="s">
+      <c r="AK55" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="AL55" s="35" t="s">
+      <c r="AL55" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="AM55" s="31"/>
-      <c r="AN55" s="31"/>
+      <c r="AM55" s="33"/>
+      <c r="AN55" s="33"/>
     </row>
     <row r="56" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D56" t="s">
@@ -4754,10 +4778,10 @@
       <c r="AA56" s="10"/>
       <c r="AB56" s="9"/>
       <c r="AE56" s="10"/>
-      <c r="AH56" s="33"/>
-      <c r="AI56" s="36"/>
-      <c r="AK56" s="34"/>
-      <c r="AL56" s="37"/>
+      <c r="AH56" s="35"/>
+      <c r="AI56" s="38"/>
+      <c r="AK56" s="36"/>
+      <c r="AL56" s="39"/>
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D57" t="s">
@@ -4788,10 +4812,14 @@
       <c r="AA57" s="18"/>
       <c r="AB57" s="19"/>
       <c r="AE57" s="10"/>
-      <c r="AH57" s="34"/>
-      <c r="AI57" s="37"/>
-      <c r="AK57" s="23"/>
-      <c r="AL57" s="24"/>
+      <c r="AH57" s="36"/>
+      <c r="AI57" s="39"/>
+      <c r="AK57" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL57" s="31">
+        <v>27</v>
+      </c>
       <c r="AM57" s="23"/>
       <c r="AN57" s="23"/>
     </row>
@@ -4830,17 +4858,21 @@
       <c r="AI58" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AJ58" s="30" t="s">
+      <c r="AJ58" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="AK58" s="23"/>
-      <c r="AL58" s="24"/>
+      <c r="AK58" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL58" s="31">
+        <v>3</v>
+      </c>
       <c r="AM58" s="23"/>
       <c r="AN58" s="23"/>
     </row>
     <row r="59" spans="1:45" x14ac:dyDescent="0.4">
       <c r="AE59" s="10"/>
-      <c r="AJ59" s="30"/>
+      <c r="AJ59" s="32"/>
       <c r="AK59" s="23"/>
       <c r="AL59" s="24"/>
       <c r="AM59" s="23"/>
@@ -4848,19 +4880,19 @@
     </row>
     <row r="60" spans="1:45" x14ac:dyDescent="0.4">
       <c r="AE60" s="10"/>
-      <c r="AJ60" s="30"/>
+      <c r="AJ60" s="32"/>
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.4">
       <c r="AE61" s="10"/>
-      <c r="AJ61" s="30"/>
+      <c r="AJ61" s="32"/>
     </row>
     <row r="62" spans="1:45" x14ac:dyDescent="0.4">
       <c r="AE62" s="10"/>
-      <c r="AJ62" s="30"/>
+      <c r="AJ62" s="32"/>
     </row>
     <row r="63" spans="1:45" x14ac:dyDescent="0.4">
       <c r="AE63" s="10"/>
-      <c r="AJ63" s="30"/>
+      <c r="AJ63" s="32"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>

</xml_diff>

<commit_message>
Nonsample other is now in the output again!
</commit_message>
<xml_diff>
--- a/worklist_template0821.xlsx
+++ b/worklist_template0821.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01c1829094dbd390/Desktop/Kelly_Lab/.venv/worklist_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{C7C7E8BA-5CC4-4271-B611-C0C6CADF7678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E6F9BAE-57F7-4610-A78F-0F18A95C5C8E}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{C7C7E8BA-5CC4-4271-B611-C0C6CADF7678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC927630-DBAD-4BC4-98F2-F02A373D0A30}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{12DA0CF9-A1F3-4B47-B73A-18ED55D7EBC7}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Manager" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="74">
   <si>
     <t>Number:</t>
   </si>
@@ -256,6 +257,9 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>QC between:</t>
   </si>
 </sst>
 </file>
@@ -3924,10 +3928,10 @@
   <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="45" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M32" sqref="M32"/>
+      <selection pane="bottomRight" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -3983,6 +3987,9 @@
       <c r="O1" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="P1" s="11" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" s="12">
@@ -4698,7 +4705,7 @@
       <c r="N16" s="12"/>
       <c r="O16" s="11"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -4744,7 +4751,7 @@
       <c r="N17" s="12"/>
       <c r="O17" s="11"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -4790,7 +4797,7 @@
       <c r="N18" s="12"/>
       <c r="O18" s="11"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -4836,7 +4843,7 @@
       <c r="N19" s="12"/>
       <c r="O19" s="11"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -4882,7 +4889,7 @@
       <c r="N20" s="12"/>
       <c r="O20" s="11"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -4928,7 +4935,7 @@
       <c r="N21" s="12"/>
       <c r="O21" s="11"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -4974,7 +4981,7 @@
       <c r="N22" s="12"/>
       <c r="O22" s="11"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" s="12">
         <v>22</v>
       </c>
@@ -5020,7 +5027,7 @@
       <c r="N23" s="12"/>
       <c r="O23" s="11"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" s="12">
         <v>23</v>
       </c>
@@ -5066,7 +5073,7 @@
       <c r="N24" s="12"/>
       <c r="O24" s="11"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -5112,7 +5119,7 @@
       <c r="N25" s="12"/>
       <c r="O25" s="11"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" s="12">
         <v>25</v>
       </c>
@@ -5158,7 +5165,7 @@
       <c r="N26" s="12"/>
       <c r="O26" s="11"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" s="12">
         <v>26</v>
       </c>
@@ -5204,7 +5211,7 @@
       <c r="N27" s="12"/>
       <c r="O27" s="11"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" s="12">
         <v>27</v>
       </c>
@@ -5250,7 +5257,7 @@
       <c r="N28" s="12"/>
       <c r="O28" s="11"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" s="12">
         <v>28</v>
       </c>
@@ -5296,7 +5303,7 @@
       <c r="N29" s="12"/>
       <c r="O29" s="11"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" s="12">
         <v>29</v>
       </c>
@@ -5342,7 +5349,7 @@
       <c r="N30" s="12"/>
       <c r="O30" s="11"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" s="12">
         <v>30</v>
       </c>
@@ -5388,7 +5395,7 @@
       <c r="N31" s="12"/>
       <c r="O31" s="11"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" s="12">
         <v>31</v>
       </c>
@@ -5437,8 +5444,11 @@
       <c r="O32" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="P32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" s="12">
         <v>32</v>
       </c>
@@ -5487,8 +5497,11 @@
       <c r="O33" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="P33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34" s="12">
         <v>33</v>
       </c>
@@ -5516,7 +5529,7 @@
       <c r="N34" s="12"/>
       <c r="O34" s="11"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35" s="12">
         <v>34</v>
       </c>
@@ -5544,7 +5557,7 @@
       <c r="N35" s="12"/>
       <c r="O35" s="11"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36" s="12">
         <v>35</v>
       </c>
@@ -5571,7 +5584,7 @@
       <c r="N36" s="12"/>
       <c r="O36" s="11"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A37" s="12">
         <v>36</v>
       </c>
@@ -5599,7 +5612,7 @@
       <c r="N37" s="12"/>
       <c r="O37" s="11"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38" s="12">
         <v>37</v>
       </c>
@@ -5627,7 +5640,7 @@
       <c r="N38" s="12"/>
       <c r="O38" s="11"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A39" s="12">
         <v>38</v>
       </c>
@@ -5655,7 +5668,7 @@
       <c r="N39" s="12"/>
       <c r="O39" s="11"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40" s="12">
         <v>39</v>
       </c>
@@ -5683,7 +5696,7 @@
       <c r="N40" s="12"/>
       <c r="O40" s="11"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A41" s="12">
         <v>40</v>
       </c>
@@ -5711,7 +5724,7 @@
       <c r="N41" s="12"/>
       <c r="O41" s="11"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42" s="12">
         <v>41</v>
       </c>
@@ -5739,7 +5752,7 @@
       <c r="N42" s="12"/>
       <c r="O42" s="11"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" s="12">
         <v>42</v>
       </c>
@@ -5767,7 +5780,7 @@
       <c r="N43" s="12"/>
       <c r="O43" s="11"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44" s="12">
         <v>43</v>
       </c>
@@ -5795,7 +5808,7 @@
       <c r="N44" s="12"/>
       <c r="O44" s="11"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45" s="12">
         <v>44</v>
       </c>
@@ -5823,7 +5836,7 @@
       <c r="N45" s="12"/>
       <c r="O45" s="11"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A46" s="12">
         <v>45</v>
       </c>
@@ -5851,7 +5864,7 @@
       <c r="N46" s="12"/>
       <c r="O46" s="11"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A47" s="12">
         <v>46</v>
       </c>
@@ -5879,7 +5892,7 @@
       <c r="N47" s="12"/>
       <c r="O47" s="11"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A48" s="12">
         <v>47</v>
       </c>

</xml_diff>